<commit_message>
-Stocks work again, but need refinement.
</commit_message>
<xml_diff>
--- a/docs/Trade Book.xlsx
+++ b/docs/Trade Book.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e32f524f1a4e77be/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monic\Actual Drive Storage\HMM_Model\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="390" documentId="8_{FEC01B4F-8B9B-4814-B62C-7C5A35FB8E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{323C2947-66DE-4940-85C1-C5AD956557E7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710CAD96-7DC3-49D6-B73B-4C041461A33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{F9CD390B-0A01-47B7-BDF5-E6BC65E8291D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{F9CD390B-0A01-47B7-BDF5-E6BC65E8291D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,10 +37,11 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+  <metadataTypes count="2">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="17">
+  <futureMetadata name="XLRICHVALUE" count="33">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -160,8 +161,134 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="53"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="56"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="59"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="62"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="65"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="68"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="71"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="74"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="77"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="80"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="83"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="86"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="89"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="92"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="95"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="98"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="17">
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </cellMetadata>
+  <valueMetadata count="33">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -212,13 +339,61 @@
     </bk>
     <bk>
       <rc t="1" v="16"/>
+    </bk>
+    <bk>
+      <rc t="1" v="17"/>
+    </bk>
+    <bk>
+      <rc t="1" v="18"/>
+    </bk>
+    <bk>
+      <rc t="1" v="19"/>
+    </bk>
+    <bk>
+      <rc t="1" v="20"/>
+    </bk>
+    <bk>
+      <rc t="1" v="21"/>
+    </bk>
+    <bk>
+      <rc t="1" v="22"/>
+    </bk>
+    <bk>
+      <rc t="1" v="23"/>
+    </bk>
+    <bk>
+      <rc t="1" v="24"/>
+    </bk>
+    <bk>
+      <rc t="1" v="25"/>
+    </bk>
+    <bk>
+      <rc t="1" v="26"/>
+    </bk>
+    <bk>
+      <rc t="1" v="27"/>
+    </bk>
+    <bk>
+      <rc t="1" v="28"/>
+    </bk>
+    <bk>
+      <rc t="1" v="29"/>
+    </bk>
+    <bk>
+      <rc t="1" v="30"/>
+    </bk>
+    <bk>
+      <rc t="1" v="31"/>
+    </bk>
+    <bk>
+      <rc t="1" v="32"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="87">
   <si>
     <t>Equities</t>
   </si>
@@ -473,6 +648,12 @@
   </si>
   <si>
     <t>Cash:</t>
+  </si>
+  <si>
+    <t>Share Diff</t>
+  </si>
+  <si>
+    <t>$ Diff</t>
   </si>
 </sst>
 </file>
@@ -482,7 +663,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -515,6 +696,19 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -643,11 +837,8 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -667,9 +858,6 @@
     <xf numFmtId="44" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -680,9 +868,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -703,12 +888,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -717,28 +896,50 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -751,21 +952,58 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1818,7 +2056,7 @@
       <xdr:rowOff>217883</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>738186</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>178594</xdr:rowOff>
@@ -1952,7 +2190,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="51">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="99">
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1vvec&amp;q=XNAS%3aIUSG&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
@@ -1997,6 +2235,49 @@
     <v>1</v>
   </rv>
   <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a22xh7&amp;q=XNAS%3aSHV&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>en-US</v>
+    <v>a22xh7</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>0</v>
+    <v>iShares:Sh Trs Bd ETF (XNAS:SHV)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>110.64</v>
+    <v>109.91</v>
+    <v>1.2035</v>
+    <v>0.04</v>
+    <v>3.634E-4</v>
+    <v>USD</v>
+    <v>Nasdaq Stock Market</v>
+    <v>XNAS</v>
+    <v>1.5E-3</v>
+    <v>110.13</v>
+    <v>ETF</v>
+    <v>45841.86940091406</v>
+    <v>3</v>
+    <v>110.11</v>
+    <v>20673158872.959999</v>
+    <v>iShares:Sh Trs Bd ETF</v>
+    <v>110.125</v>
+    <v>110.07</v>
+    <v>110.11</v>
+    <v>SHV</v>
+    <v>iShares:Sh Trs Bd ETF (XNAS:SHV)</v>
+    <v>1596521</v>
+    <v>2980289</v>
+  </rv>
+  <rv s="2">
+    <v>4</v>
+  </rv>
+  <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1vvh7&amp;q=XNAS%3aIUSV&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
@@ -2024,7 +2305,7 @@
     <v>96.49</v>
     <v>ETF</v>
     <v>45841.851699421095</v>
-    <v>3</v>
+    <v>6</v>
     <v>95.96</v>
     <v>20904088107.860001</v>
     <v>iShares:Core S&amp;P US Val</v>
@@ -2037,7 +2318,50 @@
     <v>574503</v>
   </rv>
   <rv s="2">
+    <v>7</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a22xmw&amp;q=XNAS%3aSHY&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>en-US</v>
+    <v>a22xmw</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>0</v>
+    <v>iShares:1-3 Trs Bd ETF (XNAS:SHY)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
     <v>4</v>
+    <v>83.3</v>
+    <v>81.41</v>
+    <v>1.0313000000000001</v>
+    <v>-0.09</v>
+    <v>-1.091E-3</v>
+    <v>USD</v>
+    <v>Nasdaq Stock Market</v>
+    <v>XNAS</v>
+    <v>1.5E-3</v>
+    <v>82.43</v>
+    <v>ETF</v>
+    <v>45841.839426099221</v>
+    <v>9</v>
+    <v>82.38</v>
+    <v>23975554985.849998</v>
+    <v>iShares:1-3 Trs Bd ETF</v>
+    <v>82.42</v>
+    <v>82.5</v>
+    <v>82.41</v>
+    <v>SHY</v>
+    <v>iShares:1-3 Trs Bd ETF (XNAS:SHY)</v>
+    <v>2781537</v>
+    <v>3253957</v>
+  </rv>
+  <rv s="2">
+    <v>10</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1rqkr&amp;q=BATS%3aEFG&amp;form=skydnc</v>
@@ -2067,7 +2391,7 @@
     <v>111.6</v>
     <v>ETF</v>
     <v>45841.875018448438</v>
-    <v>6</v>
+    <v>12</v>
     <v>111.21</v>
     <v>13178144921.200001</v>
     <v>iShares:MSCI EAFE Gro</v>
@@ -2080,7 +2404,50 @@
     <v>706471</v>
   </rv>
   <rv s="2">
-    <v>7</v>
+    <v>13</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1oopr&amp;q=XNAS%3aBND&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>en-US</v>
+    <v>a1oopr</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>0</v>
+    <v>Vanguard Tot Bd;ETF (XNAS:BND)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>75.67</v>
+    <v>71.1023</v>
+    <v>0.98550000000000004</v>
+    <v>-0.18</v>
+    <v>-2.457E-3</v>
+    <v>USD</v>
+    <v>Nasdaq Stock Market</v>
+    <v>XNAS</v>
+    <v>2.9999999999999997E-4</v>
+    <v>73.17</v>
+    <v>ETF</v>
+    <v>45841.873810126563</v>
+    <v>15</v>
+    <v>73.040000000000006</v>
+    <v>131369426028.83</v>
+    <v>Vanguard Tot Bd;ETF</v>
+    <v>73.13</v>
+    <v>73.260000000000005</v>
+    <v>73.08</v>
+    <v>BND</v>
+    <v>Vanguard Tot Bd;ETF (XNAS:BND)</v>
+    <v>6428422</v>
+    <v>6898741</v>
+  </rv>
+  <rv s="2">
+    <v>16</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1rrec&amp;q=BATS%3aEFV&amp;form=skydnc</v>
@@ -2110,7 +2477,7 @@
     <v>64.09</v>
     <v>ETF</v>
     <v>45841.875018008592</v>
-    <v>9</v>
+    <v>18</v>
     <v>63.87</v>
     <v>26008981758.490002</v>
     <v>iShares:MSCI EAFE Val</v>
@@ -2123,7 +2490,50 @@
     <v>3098711</v>
   </rv>
   <rv s="2">
-    <v>10</v>
+    <v>19</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1oovh&amp;q=XNAS%3aBNDX&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>en-US</v>
+    <v>a1oovh</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>0</v>
+    <v>Vanguard Tot Itl BI;ETF (XNAS:BNDX)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>50.6999</v>
+    <v>48.29</v>
+    <v>0.97619999999999996</v>
+    <v>0.08</v>
+    <v>1.6230000000000001E-3</v>
+    <v>USD</v>
+    <v>Nasdaq Stock Market</v>
+    <v>XNAS</v>
+    <v>7.000000000000001E-4</v>
+    <v>49.38</v>
+    <v>ETF</v>
+    <v>45841.838589328123</v>
+    <v>21</v>
+    <v>49.31</v>
+    <v>67518027682.480003</v>
+    <v>Vanguard Tot Itl BI;ETF</v>
+    <v>49.31</v>
+    <v>49.29</v>
+    <v>49.37</v>
+    <v>BNDX</v>
+    <v>Vanguard Tot Itl BI;ETF (XNAS:BNDX)</v>
+    <v>3923535</v>
+    <v>3827572</v>
+  </rv>
+  <rv s="2">
+    <v>22</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1vxfr&amp;q=ARCX%3aIWM&amp;form=skydnc</v>
@@ -2153,7 +2563,7 @@
     <v>223.33</v>
     <v>ETF</v>
     <v>45841.875001180466</v>
-    <v>12</v>
+    <v>24</v>
     <v>221.77</v>
     <v>63275401704.989998</v>
     <v>iShares:Russ 2000 ETF</v>
@@ -2166,7 +2576,50 @@
     <v>34272874</v>
   </rv>
   <rv s="2">
-    <v>13</v>
+    <v>25</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1rvsm&amp;q=XNAS%3aEMB&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>en-US</v>
+    <v>a1rvsm</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>0</v>
+    <v>iShares:JPM USD EM Bd (XNAS:EMB)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>93.702200000000005</v>
+    <v>84.78</v>
+    <v>1.1073</v>
+    <v>0.16</v>
+    <v>1.7330000000000002E-3</v>
+    <v>USD</v>
+    <v>Nasdaq Stock Market</v>
+    <v>XNAS</v>
+    <v>3.9000000000000003E-3</v>
+    <v>92.58</v>
+    <v>ETF</v>
+    <v>45841.839403853905</v>
+    <v>27</v>
+    <v>92.19</v>
+    <v>13685120238.15</v>
+    <v>iShares:JPM USD EM Bd</v>
+    <v>92.25</v>
+    <v>92.33</v>
+    <v>92.49</v>
+    <v>EMB</v>
+    <v>iShares:JPM USD EM Bd (XNAS:EMB)</v>
+    <v>3216935</v>
+    <v>6360992</v>
+  </rv>
+  <rv s="2">
+    <v>28</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a22pbh&amp;q=XNAS%3aSCZ&amp;form=skydnc</v>
@@ -2196,7 +2649,7 @@
     <v>73.094999999999999</v>
     <v>ETF</v>
     <v>45841.814363240628</v>
-    <v>15</v>
+    <v>30</v>
     <v>72.84</v>
     <v>10452215272.639999</v>
     <v>iShares:MSCI EAFE Sm-Cp</v>
@@ -2209,7 +2662,50 @@
     <v>989125</v>
   </rv>
   <rv s="2">
-    <v>16</v>
+    <v>31</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1x43m&amp;q=ARCX%3aLQD&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>en-US</v>
+    <v>a1x43m</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>0</v>
+    <v>iShares:iBoxx $IG Corp (ARCX:LQD)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>114.07</v>
+    <v>103.45</v>
+    <v>1.2708999999999999</v>
+    <v>-0.26</v>
+    <v>-2.3779999999999999E-3</v>
+    <v>USD</v>
+    <v>NYSE Arca</v>
+    <v>ARCX</v>
+    <v>1.4000000000000002E-3</v>
+    <v>109.28</v>
+    <v>ETF</v>
+    <v>45841.875000022657</v>
+    <v>33</v>
+    <v>108.98</v>
+    <v>29955109160.880001</v>
+    <v>iShares:iBoxx $IG Corp</v>
+    <v>109.15</v>
+    <v>109.32</v>
+    <v>109.06</v>
+    <v>LQD</v>
+    <v>iShares:iBoxx $IG Corp (ARCX:LQD)</v>
+    <v>17340488</v>
+    <v>27967093</v>
+  </rv>
+  <rv s="2">
+    <v>34</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1rp4c&amp;q=ARCX%3aEEMS&amp;form=skydnc</v>
@@ -2239,7 +2735,7 @@
     <v>65.308499999999995</v>
     <v>ETF</v>
     <v>45841.875001168752</v>
-    <v>18</v>
+    <v>36</v>
     <v>64.95</v>
     <v>380317743.18000001</v>
     <v>iShares:MSCI Em Mkt SC</v>
@@ -2252,7 +2748,50 @@
     <v>31065</v>
   </rv>
   <rv s="2">
-    <v>19</v>
+    <v>37</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1v7bh&amp;q=ARCX%3aIBND&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>en-US</v>
+    <v>a1v7bh</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>0</v>
+    <v>SPDR Bbg Intl Corp Bd (ARCX:IBND)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>32.67</v>
+    <v>27.69</v>
+    <v>0.873</v>
+    <v>0</v>
+    <v>0</v>
+    <v>USD</v>
+    <v>NYSE Arca</v>
+    <v>ARCX</v>
+    <v>5.0000000000000001E-3</v>
+    <v>32.658999999999999</v>
+    <v>ETF</v>
+    <v>45841.875000057815</v>
+    <v>39</v>
+    <v>32.42</v>
+    <v>378592906.51999998</v>
+    <v>SPDR Bbg Intl Corp Bd</v>
+    <v>32.42</v>
+    <v>32.47</v>
+    <v>32.47</v>
+    <v>IBND</v>
+    <v>SPDR Bbg Intl Corp Bd (ARCX:IBND)</v>
+    <v>43946</v>
+    <v>155980</v>
+  </rv>
+  <rv s="2">
+    <v>40</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1vyhw&amp;q=ARCX%3aIXN&amp;form=skydnc</v>
@@ -2282,7 +2821,7 @@
     <v>93.689899999999994</v>
     <v>ETF</v>
     <v>45841.875000022657</v>
-    <v>21</v>
+    <v>42</v>
     <v>92.68</v>
     <v>5530670662.96</v>
     <v>iShares:Glbl Tech</v>
@@ -2295,7 +2834,50 @@
     <v>163389</v>
   </rv>
   <rv s="2">
-    <v>22</v>
+    <v>43</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1pgqh&amp;q=BATS%3aCEMB&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>en-US</v>
+    <v>a1pgqh</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>0</v>
+    <v>iShares:JPM EM Corp Bd (BATS:CEMB)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>5</v>
+    <v>46.15</v>
+    <v>43.28</v>
+    <v>0.73109999999999997</v>
+    <v>0.01</v>
+    <v>2.2100000000000001E-4</v>
+    <v>USD</v>
+    <v>CBOE BZX Exchange</v>
+    <v>BATS</v>
+    <v>5.0000000000000001E-3</v>
+    <v>45.26</v>
+    <v>ETF</v>
+    <v>45841.875013367971</v>
+    <v>45</v>
+    <v>45.17</v>
+    <v>379810041.29000002</v>
+    <v>iShares:JPM EM Corp Bd</v>
+    <v>45.17</v>
+    <v>45.25</v>
+    <v>45.26</v>
+    <v>CEMB</v>
+    <v>iShares:JPM EM Corp Bd (BATS:CEMB)</v>
+    <v>46080</v>
+    <v>29367</v>
+  </rv>
+  <rv s="2">
+    <v>46</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a22dec&amp;q=ARCX%3aRXI&amp;form=skydnc</v>
@@ -2325,7 +2907,7 @@
     <v>190.58279999999999</v>
     <v>ETF</v>
     <v>45841.875001180466</v>
-    <v>24</v>
+    <v>48</v>
     <v>190.54</v>
     <v>254232732.65000001</v>
     <v>iShares:Glbl Con Disc</v>
@@ -2338,7 +2920,50 @@
     <v>4848</v>
   </rv>
   <rv s="2">
-    <v>25</v>
+    <v>49</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1v1r7&amp;q=ARCX%3aHYG&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>en-US</v>
+    <v>a1v1r7</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>0</v>
+    <v>iShares:iBoxx $HY Corp (ARCX:HYG)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>80.67</v>
+    <v>75.08</v>
+    <v>1.0838000000000001</v>
+    <v>0.05</v>
+    <v>6.2250000000000001E-4</v>
+    <v>USD</v>
+    <v>NYSE Arca</v>
+    <v>ARCX</v>
+    <v>4.8999999999999998E-3</v>
+    <v>80.385000000000005</v>
+    <v>ETF</v>
+    <v>45841.875000046093</v>
+    <v>51</v>
+    <v>80.260000000000005</v>
+    <v>17748842610.57</v>
+    <v>iShares:iBoxx $HY Corp</v>
+    <v>80.3</v>
+    <v>80.319999999999993</v>
+    <v>80.37</v>
+    <v>HYG</v>
+    <v>iShares:iBoxx $HY Corp (ARCX:HYG)</v>
+    <v>19749999</v>
+    <v>35257306</v>
+  </rv>
+  <rv s="2">
+    <v>52</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1vykr&amp;q=ARCX%3aIXP&amp;form=skydnc</v>
@@ -2368,7 +2993,7 @@
     <v>111.64</v>
     <v>ETF</v>
     <v>45841.875001122658</v>
-    <v>27</v>
+    <v>54</v>
     <v>111.34</v>
     <v>538498562.48000002</v>
     <v>iShares:Glbl Comm Svcs</v>
@@ -2381,7 +3006,50 @@
     <v>44571</v>
   </rv>
   <rv s="2">
-    <v>28</v>
+    <v>55</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1v32w&amp;q=BATS%3aHYXU&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>en-US</v>
+    <v>a1v32w</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>0</v>
+    <v>iShares:Internatl HY Bd (BATS:HYXU)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>5</v>
+    <v>55.1</v>
+    <v>45.76</v>
+    <v>1.2275</v>
+    <v>-0.06</v>
+    <v>-1.0889999999999999E-3</v>
+    <v>USD</v>
+    <v>CBOE BZX Exchange</v>
+    <v>BATS</v>
+    <v>4.0000000000000001E-3</v>
+    <v>55.1</v>
+    <v>ETF</v>
+    <v>45841.875031921096</v>
+    <v>57</v>
+    <v>54.94</v>
+    <v>49117437.090000004</v>
+    <v>iShares:Internatl HY Bd</v>
+    <v>55.1</v>
+    <v>55.08</v>
+    <v>55.02</v>
+    <v>HYXU</v>
+    <v>iShares:Internatl HY Bd (BATS:HYXU)</v>
+    <v>11575</v>
+    <v>10902</v>
+  </rv>
+  <rv s="2">
+    <v>58</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1vy9c&amp;q=ARCX%3aIXC&amp;form=skydnc</v>
@@ -2411,7 +3079,7 @@
     <v>40.24</v>
     <v>ETF</v>
     <v>45841.875000034372</v>
-    <v>30</v>
+    <v>60</v>
     <v>40.08</v>
     <v>1729483357.02</v>
     <v>iShares:Glbl Energy</v>
@@ -2424,7 +3092,50 @@
     <v>454262</v>
   </rv>
   <rv s="2">
-    <v>31</v>
+    <v>61</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1rwxm&amp;q=BATS%3aEMHY&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>en-US</v>
+    <v>a1rwxm</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>0</v>
+    <v>iShares:JPM EM Hi Yld Bd (BATS:EMHY)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>5</v>
+    <v>39.07</v>
+    <v>35.784999999999997</v>
+    <v>0.95230000000000004</v>
+    <v>0.12</v>
+    <v>3.0959999999999998E-3</v>
+    <v>USD</v>
+    <v>CBOE BZX Exchange</v>
+    <v>BATS</v>
+    <v>5.0000000000000001E-3</v>
+    <v>38.909999999999997</v>
+    <v>ETF</v>
+    <v>45841.875022418753</v>
+    <v>63</v>
+    <v>38.76</v>
+    <v>434276730.26999998</v>
+    <v>iShares:JPM EM Hi Yld Bd</v>
+    <v>38.76</v>
+    <v>38.76</v>
+    <v>38.880000000000003</v>
+    <v>EMHY</v>
+    <v>iShares:JPM EM Hi Yld Bd (BATS:EMHY)</v>
+    <v>16864</v>
+    <v>57244</v>
+  </rv>
+  <rv s="2">
+    <v>64</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1y6vh&amp;q=ARCX%3aMXI&amp;form=skydnc</v>
@@ -2454,7 +3165,7 @@
     <v>87.93</v>
     <v>ETF</v>
     <v>45841.875000034372</v>
-    <v>33</v>
+    <v>66</v>
     <v>87.67</v>
     <v>222393986.11000001</v>
     <v>iShares:Glbl Materials</v>
@@ -2467,7 +3178,50 @@
     <v>7557</v>
   </rv>
   <rv s="2">
-    <v>34</v>
+    <v>67</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1vbbh&amp;q=XNAS%3aIEF&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>en-US</v>
+    <v>a1vbbh</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>0</v>
+    <v>iShares:7-10 Trs Bd (XNAS:IEF)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>99.18</v>
+    <v>91.08</v>
+    <v>1.1986000000000001</v>
+    <v>-0.33</v>
+    <v>-3.4699999999999996E-3</v>
+    <v>USD</v>
+    <v>Nasdaq Stock Market</v>
+    <v>XNAS</v>
+    <v>1.5E-3</v>
+    <v>94.86</v>
+    <v>ETF</v>
+    <v>45841.861515983597</v>
+    <v>69</v>
+    <v>94.635000000000005</v>
+    <v>34991153010.519997</v>
+    <v>iShares:7-10 Trs Bd</v>
+    <v>94.8</v>
+    <v>95.09</v>
+    <v>94.76</v>
+    <v>IEF</v>
+    <v>iShares:7-10 Trs Bd (XNAS:IEF)</v>
+    <v>7398883</v>
+    <v>8162986</v>
+  </rv>
+  <rv s="2">
+    <v>70</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1vyc7&amp;q=ARCX%3aIXG&amp;form=skydnc</v>
@@ -2497,7 +3251,7 @@
     <v>112.2242</v>
     <v>ETF</v>
     <v>45841.87500115703</v>
-    <v>36</v>
+    <v>72</v>
     <v>111.49</v>
     <v>527139109.95999998</v>
     <v>iShares:Glbl Financials</v>
@@ -2510,7 +3264,50 @@
     <v>15707</v>
   </rv>
   <rv s="2">
-    <v>37</v>
+    <v>73</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a24b5r&amp;q=XNAS%3aTLT&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>en-US</v>
+    <v>a24b5r</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>0</v>
+    <v>iShares:20+ Trs Bd ETF (XNAS:TLT)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>101.64</v>
+    <v>83.295000000000002</v>
+    <v>1.0688</v>
+    <v>-0.61</v>
+    <v>-6.9649999999999998E-3</v>
+    <v>USD</v>
+    <v>Nasdaq Stock Market</v>
+    <v>XNAS</v>
+    <v>1.5E-3</v>
+    <v>87.29</v>
+    <v>ETF</v>
+    <v>45841.873756284374</v>
+    <v>75</v>
+    <v>86.85</v>
+    <v>48945400501.349998</v>
+    <v>iShares:20+ Trs Bd ETF</v>
+    <v>87.165000000000006</v>
+    <v>87.58</v>
+    <v>86.97</v>
+    <v>TLT</v>
+    <v>iShares:20+ Trs Bd ETF (XNAS:TLT)</v>
+    <v>26729101</v>
+    <v>39419697</v>
+  </rv>
+  <rv s="2">
+    <v>76</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1shxm&amp;q=ARCX%3aEXI&amp;form=skydnc</v>
@@ -2540,7 +3337,7 @@
     <v>166.16</v>
     <v>ETF</v>
     <v>45841.875000010936</v>
-    <v>39</v>
+    <v>78</v>
     <v>165.5</v>
     <v>949777609.61000001</v>
     <v>iShares:Glbl Industrials</v>
@@ -2553,7 +3350,50 @@
     <v>29453</v>
   </rv>
   <rv s="2">
-    <v>40</v>
+    <v>79</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1u477&amp;q=BATS%3aGOVT&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>en-US</v>
+    <v>a1u477</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>0</v>
+    <v>iShares:US Treasury Bond (BATS:GOVT)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>5</v>
+    <v>23.689</v>
+    <v>22.23</v>
+    <v>0.88759999999999994</v>
+    <v>-0.06</v>
+    <v>-2.627E-3</v>
+    <v>USD</v>
+    <v>CBOE BZX Exchange</v>
+    <v>BATS</v>
+    <v>5.0000000000000001E-4</v>
+    <v>22.8</v>
+    <v>ETF</v>
+    <v>45841.875029594528</v>
+    <v>81</v>
+    <v>22.76</v>
+    <v>27551902585.279999</v>
+    <v>iShares:US Treasury Bond</v>
+    <v>22.79</v>
+    <v>22.84</v>
+    <v>22.78</v>
+    <v>GOVT</v>
+    <v>iShares:US Treasury Bond (BATS:GOVT)</v>
+    <v>6171454</v>
+    <v>9143840</v>
+  </rv>
+  <rv s="2">
+    <v>82</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1vyf2&amp;q=ARCX%3aIXJ&amp;form=skydnc</v>
@@ -2583,7 +3423,7 @@
     <v>86.54</v>
     <v>ETF</v>
     <v>45841.875000022657</v>
-    <v>42</v>
+    <v>84</v>
     <v>86.08</v>
     <v>3754328855.6100001</v>
     <v>iShares:Glbl HealthCare</v>
@@ -2596,7 +3436,50 @@
     <v>179543</v>
   </rv>
   <rv s="2">
-    <v>43</v>
+    <v>85</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1ve9c&amp;q=XNAS%3aIGOV&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>en-US</v>
+    <v>a1ve9c</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>0</v>
+    <v>iShares:Itl Trs Bd (XNAS:IGOV)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>43.33</v>
+    <v>37.299999999999997</v>
+    <v>0.93710000000000004</v>
+    <v>-0.04</v>
+    <v>-9.2869999999999997E-4</v>
+    <v>USD</v>
+    <v>Nasdaq Stock Market</v>
+    <v>XNAS</v>
+    <v>3.4999999999999996E-3</v>
+    <v>43.07</v>
+    <v>ETF</v>
+    <v>45841.870283981247</v>
+    <v>87</v>
+    <v>42.9</v>
+    <v>1209512469.77</v>
+    <v>iShares:Itl Trs Bd</v>
+    <v>43.07</v>
+    <v>43.07</v>
+    <v>43.03</v>
+    <v>IGOV</v>
+    <v>iShares:Itl Trs Bd (XNAS:IGOV)</v>
+    <v>267387</v>
+    <v>466808</v>
+  </rv>
+  <rv s="2">
+    <v>88</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1wpjc&amp;q=ARCX%3aKXI&amp;form=skydnc</v>
@@ -2626,7 +3509,7 @@
     <v>66.075000000000003</v>
     <v>ETF</v>
     <v>45841.875000034372</v>
-    <v>45</v>
+    <v>90</v>
     <v>65.8</v>
     <v>856595533.98000002</v>
     <v>iShares:Glbl Con Staples</v>
@@ -2639,7 +3522,50 @@
     <v>78105</v>
   </rv>
   <rv s="2">
-    <v>46</v>
+    <v>91</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a25nkr&amp;q=XNAS%3aVWOB&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>en-US</v>
+    <v>a25nkr</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>0</v>
+    <v>Vanguard EM G B;ETF (XNAS:VWOB)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>66.647599999999997</v>
+    <v>60.905000000000001</v>
+    <v>1.0858000000000001</v>
+    <v>0.06</v>
+    <v>9.2050000000000009E-4</v>
+    <v>USD</v>
+    <v>Nasdaq Stock Market</v>
+    <v>XNAS</v>
+    <v>1.5E-3</v>
+    <v>65.305000000000007</v>
+    <v>ETF</v>
+    <v>45841.838592117965</v>
+    <v>93</v>
+    <v>65.099599999999995</v>
+    <v>5200391640.3199997</v>
+    <v>Vanguard EM G B;ETF</v>
+    <v>65.11</v>
+    <v>65.180000000000007</v>
+    <v>65.239999999999995</v>
+    <v>VWOB</v>
+    <v>Vanguard EM G B;ETF (XNAS:VWOB)</v>
+    <v>308360</v>
+    <v>406780</v>
+  </rv>
+  <rv s="2">
+    <v>94</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1wddm&amp;q=ARCX%3aJXI&amp;form=skydnc</v>
@@ -2669,7 +3595,7 @@
     <v>73.89</v>
     <v>ETF</v>
     <v>45841.875001180466</v>
-    <v>48</v>
+    <v>96</v>
     <v>73.459999999999994</v>
     <v>187766460.78999999</v>
     <v>iShares:Glbl Utilities</v>
@@ -2682,7 +3608,7 @@
     <v>12453</v>
   </rv>
   <rv s="2">
-    <v>49</v>
+    <v>97</v>
   </rv>
 </rvData>
 </file>
@@ -3247,1663 +4173,1847 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF4EA2D-A99D-466C-9550-F90D9897FACD}">
-  <dimension ref="A1:AB28"/>
+  <dimension ref="A1:AD28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="24" customWidth="1"/>
-    <col min="4" max="7" width="20.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="28" customWidth="1"/>
-    <col min="9" max="12" width="20.7109375" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" style="28" customWidth="1"/>
-    <col min="14" max="17" width="20.7109375" customWidth="1"/>
-    <col min="18" max="18" width="20.7109375" style="28" customWidth="1"/>
-    <col min="19" max="27" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="21" customWidth="1"/>
+    <col min="4" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="23" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="23" customWidth="1"/>
+    <col min="11" max="15" width="20.7109375" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" style="23" customWidth="1"/>
+    <col min="17" max="20" width="20.7109375" customWidth="1"/>
+    <col min="21" max="21" width="20.7109375" style="23" customWidth="1"/>
+    <col min="22" max="30" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:30" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="46" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="44" t="s">
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
       <c r="Q1" s="45"/>
-      <c r="R1" s="46" t="s">
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
-      <c r="V1" s="42"/>
-      <c r="W1" s="46" t="s">
+      <c r="V1" s="48"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="X1" s="41"/>
-      <c r="Y1" s="41"/>
-      <c r="Z1" s="41"/>
-      <c r="AA1" s="42"/>
+      <c r="AA1" s="48"/>
+      <c r="AB1" s="48"/>
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="49"/>
     </row>
-    <row r="2" spans="1:27" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32">
+    <row r="2" spans="1:30" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="40">
         <v>50000</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="36" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="51"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="36" t="s">
+      <c r="O2" s="65"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="R2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="S2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="T2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M2" s="48"/>
-      <c r="N2" s="2" t="s">
+      <c r="U2" s="18"/>
+      <c r="V2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="W2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="X2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Y2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="R2" s="21"/>
-      <c r="S2" s="2" t="s">
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="AB2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="AC2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="AD2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="W2" s="21"/>
-      <c r="X2" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y2" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z2" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>48</v>
-      </c>
     </row>
-    <row r="3" spans="1:27" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="22" t="e" vm="1">
+    <row r="3" spans="1:30" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="41"/>
+      <c r="B3" s="19" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="5">
-        <v>0</v>
-      </c>
-      <c r="E3" s="37">
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="57">
         <f>D3*$A$2</f>
         <v>0</v>
       </c>
-      <c r="F3" s="7">
-        <v>0</v>
-      </c>
-      <c r="G3" s="47">
-        <f t="shared" ref="G3:G19" si="0">E3-F3</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="51" t="s">
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+      <c r="G3" s="50">
+        <f>E3-F3</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="61" cm="1">
+        <f t="array" aca="1" ref="H3" ca="1">G3/_FV(B3,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="52" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J3" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="5">
+      <c r="K3" s="4">
         <f>A10</f>
         <v>0</v>
       </c>
-      <c r="J3" s="50">
-        <f>I3*$A$2</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="10">
-        <v>0</v>
-      </c>
-      <c r="L3" s="11">
-        <f>J3-K3</f>
-        <v>0</v>
-      </c>
-      <c r="M3" s="49" t="s">
+      <c r="L3" s="60">
+        <f>K3*$A$2</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="9">
+        <v>0</v>
+      </c>
+      <c r="N3" s="59">
+        <f>L3-M3</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="66" cm="1">
+        <f t="array" aca="1" ref="O3" ca="1">N3/_FV(I3,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="5">
-        <v>0</v>
-      </c>
-      <c r="O3" s="6">
-        <f>N3*$A$2</f>
-        <v>0</v>
-      </c>
-      <c r="P3" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="8">
-        <f>O3-P3</f>
-        <v>0</v>
-      </c>
-      <c r="R3" s="25" t="s">
+      <c r="Q3" s="4">
+        <v>0</v>
+      </c>
+      <c r="R3" s="5">
+        <f>Q3*$A$2</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="6">
+        <v>0</v>
+      </c>
+      <c r="T3" s="7">
+        <f>R3-S3</f>
+        <v>0</v>
+      </c>
+      <c r="U3" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="S3" s="5">
-        <v>0</v>
-      </c>
-      <c r="T3" s="6">
-        <f>S3*$A$2</f>
-        <v>0</v>
-      </c>
-      <c r="U3" s="7">
-        <v>0</v>
-      </c>
-      <c r="V3" s="8">
-        <f>T3-U3</f>
-        <v>0</v>
-      </c>
-      <c r="W3" s="25" t="s">
+      <c r="V3" s="4">
+        <v>0</v>
+      </c>
+      <c r="W3" s="5">
+        <f>V3*$A$2</f>
+        <v>0</v>
+      </c>
+      <c r="X3" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="7">
+        <f>W3-X3</f>
+        <v>0</v>
+      </c>
+      <c r="Z3" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="X3" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="37">
-        <f>X3*$A$2</f>
-        <v>0</v>
-      </c>
-      <c r="Z3" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="8">
-        <f>Y3-Z3</f>
+      <c r="AA3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="5">
+        <f>AA3*$A$2</f>
+        <v>0</v>
+      </c>
+      <c r="AC3" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="7">
+        <f>AB3-AC3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="22" t="e" vm="2">
+    <row r="4" spans="1:30" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="41"/>
+      <c r="B4" s="19" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="37">
-        <f t="shared" ref="E4:E19" si="1">D4*$A$2</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="7">
-        <v>0</v>
-      </c>
-      <c r="G4" s="47">
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="57">
+        <f t="shared" ref="E4:E19" si="0">D4*$A$2</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="50">
+        <f>E4-F4</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="61" cm="1">
+        <f t="array" aca="1" ref="H4" ca="1">G4/_FV(B4,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="52" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="60">
+        <f t="shared" ref="L4:L18" si="1">K4*$A$2</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0</v>
+      </c>
+      <c r="N4" s="59">
+        <f t="shared" ref="N4:N18" si="2">L4-M4</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="66" cm="1">
+        <f t="array" aca="1" ref="O4" ca="1">N4/_FV(I4,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>0.111</v>
+      </c>
+      <c r="R4" s="5">
+        <f t="shared" ref="R4:R9" si="3">Q4*$A$2</f>
+        <v>5550</v>
+      </c>
+      <c r="S4" s="6">
+        <v>0</v>
+      </c>
+      <c r="T4" s="7">
+        <f t="shared" ref="T4:T9" si="4">R4-S4</f>
+        <v>5550</v>
+      </c>
+      <c r="U4" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" s="4">
+        <v>0</v>
+      </c>
+      <c r="W4" s="5">
+        <f t="shared" ref="W4:W8" si="5">V4*$A$2</f>
+        <v>0</v>
+      </c>
+      <c r="X4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="7">
+        <f t="shared" ref="Y4:Y8" si="6">W4-X4</f>
+        <v>0</v>
+      </c>
+      <c r="Z4" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="5">
+        <f t="shared" ref="AB4:AB19" si="7">AA4*$A$2</f>
+        <v>0</v>
+      </c>
+      <c r="AC4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="7">
+        <f t="shared" ref="AD4:AD19" si="8">AB4-AC4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="41"/>
+      <c r="B5" s="19" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="57">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H4" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0</v>
-      </c>
-      <c r="J4" s="50">
-        <f t="shared" ref="J4:J18" si="2">I4*$A$2</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="10">
-        <v>0</v>
-      </c>
-      <c r="L4" s="11">
-        <f t="shared" ref="L4:L18" si="3">J4-K4</f>
-        <v>0</v>
-      </c>
-      <c r="M4" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="5">
-        <v>0.111</v>
-      </c>
-      <c r="O4" s="6">
-        <f t="shared" ref="O4:O9" si="4">N4*$A$2</f>
-        <v>5550</v>
-      </c>
-      <c r="P4" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="8">
-        <f t="shared" ref="Q4:Q9" si="5">O4-P4</f>
-        <v>5550</v>
-      </c>
-      <c r="R4" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="S4" s="5">
-        <v>0</v>
-      </c>
-      <c r="T4" s="6">
-        <f t="shared" ref="T4:T8" si="6">S4*$A$2</f>
-        <v>0</v>
-      </c>
-      <c r="U4" s="7">
-        <v>0</v>
-      </c>
-      <c r="V4" s="8">
-        <f t="shared" ref="V4:V8" si="7">T4-U4</f>
-        <v>0</v>
-      </c>
-      <c r="W4" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="X4" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="37">
-        <f t="shared" ref="Y4:Y19" si="8">X4*$A$2</f>
-        <v>0</v>
-      </c>
-      <c r="Z4" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="8">
-        <f t="shared" ref="AA4:AA19" si="9">Y4-Z4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="22" t="e" vm="3">
+      <c r="F5" s="6"/>
+      <c r="G5" s="50">
+        <f>E5-F5</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="61" cm="1">
+        <f t="array" aca="1" ref="H5" ca="1">G5/_FV(B5,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="53" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="37">
+      <c r="J5" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0</v>
+      </c>
+      <c r="L5" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="50">
+      <c r="M5" s="9">
+        <v>0</v>
+      </c>
+      <c r="N5" s="59">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K5" s="10">
-        <v>0</v>
-      </c>
-      <c r="L5" s="11">
+      <c r="O5" s="66" cm="1">
+        <f t="array" aca="1" ref="O5" ca="1">N5/_FV(I5,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>0</v>
+      </c>
+      <c r="R5" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M5" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="N5" s="5">
-        <v>0</v>
-      </c>
-      <c r="O5" s="6">
+      <c r="S5" s="6">
+        <v>0</v>
+      </c>
+      <c r="T5" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P5" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="8">
+      <c r="U5" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="V5" s="4">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="W5" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="R5" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="S5" s="5">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="T5" s="6">
+        <v>2700</v>
+      </c>
+      <c r="X5" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="7">
         <f t="shared" si="6"/>
         <v>2700</v>
       </c>
-      <c r="U5" s="7">
-        <v>0</v>
-      </c>
-      <c r="V5" s="8">
+      <c r="Z5" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="5">
         <f t="shared" si="7"/>
-        <v>2700</v>
-      </c>
-      <c r="W5" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="X5" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="37">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="8">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:27" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="22" t="e" vm="4">
+    <row r="6" spans="1:30" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="41"/>
+      <c r="B6" s="19" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="37">
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="57">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="50">
+        <f>E6-F6</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="61" cm="1">
+        <f t="array" aca="1" ref="H6" ca="1">G6/_FV(B6,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="53" t="e" vm="8">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J6" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+      <c r="L6" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F6" s="7">
-        <v>0</v>
-      </c>
-      <c r="G6" s="47">
+      <c r="M6" s="9">
+        <v>0</v>
+      </c>
+      <c r="N6" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="66" cm="1">
+        <f t="array" aca="1" ref="O6" ca="1">N6/_FV(I6,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>0</v>
+      </c>
+      <c r="R6" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S6" s="6">
+        <v>0</v>
+      </c>
+      <c r="T6" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="U6" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="V6" s="4">
+        <v>0</v>
+      </c>
+      <c r="W6" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="X6" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z6" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AC6" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A7" s="41"/>
+      <c r="B7" s="19" t="e" vm="9">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="57">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0</v>
-      </c>
-      <c r="J6" s="50">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K6" s="10">
-        <v>0</v>
-      </c>
-      <c r="L6" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M6" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="N6" s="5">
-        <v>0</v>
-      </c>
-      <c r="O6" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P6" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="8">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="R6" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="S6" s="5">
-        <v>0</v>
-      </c>
-      <c r="T6" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U6" s="7">
-        <v>0</v>
-      </c>
-      <c r="V6" s="8">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="W6" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="X6" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="37">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="8">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="22" t="e" vm="5">
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
+      <c r="G7" s="50">
+        <f>E7-F7</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="61" cm="1">
+        <f t="array" aca="1" ref="H7" ca="1">G7/_FV(B7,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="53" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0</v>
-      </c>
-      <c r="E7" s="37">
+      <c r="J7" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0.111</v>
+      </c>
+      <c r="L7" s="60">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="7">
-        <v>0</v>
-      </c>
-      <c r="G7" s="47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0.111</v>
-      </c>
-      <c r="J7" s="50">
+        <v>5550</v>
+      </c>
+      <c r="M7" s="9">
+        <v>0</v>
+      </c>
+      <c r="N7" s="59">
         <f t="shared" si="2"/>
         <v>5550</v>
       </c>
-      <c r="K7" s="10">
-        <v>0</v>
-      </c>
-      <c r="L7" s="11">
+      <c r="O7" s="66" cm="1">
+        <f t="array" aca="1" ref="O7" ca="1">N7/_FV(I7,"Price")</f>
+        <v>60.00648718780409</v>
+      </c>
+      <c r="P7" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>0</v>
+      </c>
+      <c r="R7" s="5">
         <f t="shared" si="3"/>
-        <v>5550</v>
-      </c>
-      <c r="M7" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="N7" s="5">
-        <v>0</v>
-      </c>
-      <c r="O7" s="6">
+        <v>0</v>
+      </c>
+      <c r="S7" s="6">
+        <v>0</v>
+      </c>
+      <c r="T7" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P7" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="8">
+      <c r="U7" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="V7" s="4">
+        <v>0</v>
+      </c>
+      <c r="W7" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R7" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="S7" s="5">
-        <v>0</v>
-      </c>
-      <c r="T7" s="6">
+      <c r="X7" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="U7" s="7">
-        <v>0</v>
-      </c>
-      <c r="V7" s="8">
+      <c r="Z7" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="5">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="W7" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="X7" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="37">
+      <c r="AC7" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z7" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="8">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:27" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="22" t="e" vm="6">
+    <row r="8" spans="1:30" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="41"/>
+      <c r="B8" s="19" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="5">
-        <v>0</v>
-      </c>
-      <c r="E8" s="37">
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="57">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8" s="50">
+        <f>E8-F8</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="61" cm="1">
+        <f t="array" aca="1" ref="H8" ca="1">G8/_FV(B8,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="53" t="e" vm="12">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J8" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+      <c r="L8" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F8" s="7">
-        <v>0</v>
-      </c>
-      <c r="G8" s="47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="5">
-        <v>0</v>
-      </c>
-      <c r="J8" s="50">
+      <c r="M8" s="9">
+        <v>0</v>
+      </c>
+      <c r="N8" s="59">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K8" s="10">
-        <v>0</v>
-      </c>
-      <c r="L8" s="11">
+      <c r="O8" s="66" cm="1">
+        <f t="array" aca="1" ref="O8" ca="1">N8/_FV(I8,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="R8" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M8" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="N8" s="5">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="O8" s="6">
+        <v>3649.9999999999995</v>
+      </c>
+      <c r="S8" s="6">
+        <v>0</v>
+      </c>
+      <c r="T8" s="7">
         <f t="shared" si="4"/>
         <v>3649.9999999999995</v>
       </c>
-      <c r="P8" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="8">
+      <c r="U8" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="V8" s="10">
+        <v>0</v>
+      </c>
+      <c r="W8" s="11">
         <f t="shared" si="5"/>
-        <v>3649.9999999999995</v>
-      </c>
-      <c r="R8" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="S8" s="12">
-        <v>0</v>
-      </c>
-      <c r="T8" s="13">
+        <v>0</v>
+      </c>
+      <c r="X8" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="13">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="U8" s="14">
-        <v>0</v>
-      </c>
-      <c r="V8" s="15">
+      <c r="Z8" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="5">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="W8" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="X8" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="37">
+      <c r="AC8" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z8" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="8">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="9" spans="1:27" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:30" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="22" t="e" vm="7">
+      <c r="B9" s="19" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="5">
-        <v>0</v>
-      </c>
-      <c r="E9" s="37">
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="57">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="50">
+        <f>E9-F9</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="61" cm="1">
+        <f t="array" aca="1" ref="H9" ca="1">G9/_FV(B9,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="53" t="e" vm="14">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J9" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="4">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="L9" s="60">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="7">
-        <v>0</v>
-      </c>
-      <c r="G9" s="47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="5">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="J9" s="50">
+        <v>2900</v>
+      </c>
+      <c r="M9" s="9">
+        <v>0</v>
+      </c>
+      <c r="N9" s="59">
         <f t="shared" si="2"/>
         <v>2900</v>
       </c>
-      <c r="K9" s="10">
-        <v>0</v>
-      </c>
-      <c r="L9" s="11">
+      <c r="O9" s="66" cm="1">
+        <f t="array" aca="1" ref="O9" ca="1">N9/_FV(I9,"Price")</f>
+        <v>89.31321219587312</v>
+      </c>
+      <c r="P9" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q9" s="10">
+        <v>0</v>
+      </c>
+      <c r="R9" s="11">
         <f t="shared" si="3"/>
-        <v>2900</v>
-      </c>
-      <c r="M9" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="N9" s="12">
-        <v>0</v>
-      </c>
-      <c r="O9" s="13">
+        <v>0</v>
+      </c>
+      <c r="S9" s="12">
+        <v>0</v>
+      </c>
+      <c r="T9" s="13">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P9" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="15">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="R9" s="27"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="25" t="s">
+      <c r="U9" s="22"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="X9" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="37">
+      <c r="AA9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AC9" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="8">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="10" spans="1:27" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="33">
-        <f>1-SUM(D3:D19,I4:I18,N3:N9,S3:S8)</f>
-        <v>0</v>
-      </c>
-      <c r="B10" s="22" t="e" vm="8">
+    <row r="10" spans="1:30" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="43">
+        <f>1-SUM(D3:D19,K4:K18,Q3:Q9,V3:V8)</f>
+        <v>0</v>
+      </c>
+      <c r="B10" s="19" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="5">
-        <v>0</v>
-      </c>
-      <c r="E10" s="37">
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="57">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10" s="50">
+        <f>E10-F10</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="61" cm="1">
+        <f t="array" aca="1" ref="H10" ca="1">G10/_FV(B10,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="53" t="e" vm="16">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J10" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+      <c r="L10" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F10" s="7">
-        <v>0</v>
-      </c>
-      <c r="G10" s="47">
+      <c r="M10" s="9">
+        <v>0</v>
+      </c>
+      <c r="N10" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="66" cm="1">
+        <f t="array" aca="1" ref="O10" ca="1">N10/_FV(I10,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="22"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AC10" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A11" s="41"/>
+      <c r="B11" s="19" t="e" vm="17">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="57">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" s="5">
-        <v>0</v>
-      </c>
-      <c r="J10" s="50">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K10" s="10">
-        <v>0</v>
-      </c>
-      <c r="L10" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M10" s="27"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="27"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4"/>
-      <c r="W10" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="X10" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="37">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="8">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="22" t="e" vm="9">
+      <c r="F11" s="6">
+        <v>0</v>
+      </c>
+      <c r="G11" s="50">
+        <f>E11-F11</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="61" cm="1">
+        <f t="array" aca="1" ref="H11" ca="1">G11/_FV(B11,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="53" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
-      <c r="C11" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0</v>
-      </c>
-      <c r="E11" s="37">
+      <c r="J11" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0.111</v>
+      </c>
+      <c r="L11" s="60">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="7">
-        <v>0</v>
-      </c>
-      <c r="G11" s="47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" s="5">
-        <v>0.111</v>
-      </c>
-      <c r="J11" s="50">
+        <v>5550</v>
+      </c>
+      <c r="M11" s="9">
+        <v>0</v>
+      </c>
+      <c r="N11" s="59">
         <f t="shared" si="2"/>
         <v>5550</v>
       </c>
-      <c r="K11" s="10">
-        <v>0</v>
-      </c>
-      <c r="L11" s="11">
-        <f t="shared" si="3"/>
-        <v>5550</v>
-      </c>
-      <c r="M11" s="27"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="27"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="4"/>
-      <c r="W11" s="25" t="s">
+      <c r="O11" s="66" cm="1">
+        <f t="array" aca="1" ref="O11" ca="1">N11/_FV(I11,"Price")</f>
+        <v>69.055617767823804</v>
+      </c>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="22"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="X11" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="37">
+      <c r="AA11" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AC11" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="8">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:27" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="22" t="e" vm="10">
+    <row r="12" spans="1:30" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="19" t="e" vm="19">
         <v>#VALUE!</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="E12" s="37">
-        <f t="shared" si="1"/>
-        <v>1900</v>
-      </c>
-      <c r="F12" s="7">
-        <v>0</v>
-      </c>
-      <c r="G12" s="47">
+      <c r="E12" s="57">
         <f t="shared" si="0"/>
         <v>1900</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="F12" s="6">
+        <v>2200</v>
+      </c>
+      <c r="G12" s="50">
+        <f>E12-F12</f>
+        <v>-300</v>
+      </c>
+      <c r="H12" s="61" cm="1">
+        <f t="array" aca="1" ref="H12" ca="1">G12/_FV(B12,"Price")</f>
+        <v>-2.6872088857040488</v>
+      </c>
+      <c r="I12" s="53" t="e" vm="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J12" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="5">
-        <v>0</v>
-      </c>
-      <c r="J12" s="50">
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="60">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="9">
+        <v>0</v>
+      </c>
+      <c r="N12" s="59">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K12" s="10">
-        <v>0</v>
-      </c>
-      <c r="L12" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="27"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="27"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
-      <c r="W12" s="25" t="s">
+      <c r="O12" s="66" cm="1">
+        <f t="array" aca="1" ref="O12" ca="1">N12/_FV(I12,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="22"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="X12" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="37">
+      <c r="AA12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AC12" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z12" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="8">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="13" spans="1:27" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="22" t="e" vm="11">
+    <row r="13" spans="1:30" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="19" t="e" vm="21">
         <v>#VALUE!</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="5">
-        <v>0</v>
-      </c>
-      <c r="E13" s="37">
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="57">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0</v>
+      </c>
+      <c r="G13" s="50">
+        <f>E13-F13</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="61" cm="1">
+        <f t="array" aca="1" ref="H13" ca="1">G13/_FV(B13,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="53" t="e" vm="22">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J13" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0.111</v>
+      </c>
+      <c r="L13" s="60">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="7">
-        <v>0</v>
-      </c>
-      <c r="G13" s="47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="5">
-        <v>0.111</v>
-      </c>
-      <c r="J13" s="50">
+        <v>5550</v>
+      </c>
+      <c r="M13" s="9">
+        <v>0</v>
+      </c>
+      <c r="N13" s="59">
         <f t="shared" si="2"/>
         <v>5550</v>
       </c>
-      <c r="K13" s="10">
-        <v>0</v>
-      </c>
-      <c r="L13" s="11">
-        <f t="shared" si="3"/>
-        <v>5550</v>
-      </c>
-      <c r="M13" s="27"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
-      <c r="W13" s="25" t="s">
+      <c r="O13" s="66" cm="1">
+        <f t="array" aca="1" ref="O13" ca="1">N13/_FV(I13,"Price")</f>
+        <v>142.74691358024691</v>
+      </c>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="22"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="X13" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="37">
+      <c r="AA13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AC13" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z13" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="8">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="14" spans="1:27" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="22" t="e" vm="12">
+    <row r="14" spans="1:30" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="19" t="e" vm="23">
         <v>#VALUE!</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="E14" s="37">
-        <f t="shared" si="1"/>
-        <v>2850</v>
-      </c>
-      <c r="F14" s="7">
-        <v>0</v>
-      </c>
-      <c r="G14" s="47">
+      <c r="E14" s="57">
         <f t="shared" si="0"/>
         <v>2850</v>
       </c>
-      <c r="H14" s="25" t="s">
+      <c r="F14" s="6">
+        <v>0</v>
+      </c>
+      <c r="G14" s="50">
+        <f>E14-F14</f>
+        <v>2850</v>
+      </c>
+      <c r="H14" s="61" cm="1">
+        <f t="array" aca="1" ref="H14" ca="1">G14/_FV(B14,"Price")</f>
+        <v>32.508269647541916</v>
+      </c>
+      <c r="I14" s="53" t="e" vm="24">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J14" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="5">
-        <v>0</v>
-      </c>
-      <c r="J14" s="50">
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
+      <c r="L14" s="60">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="9">
+        <v>0</v>
+      </c>
+      <c r="N14" s="59">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K14" s="10">
-        <v>0</v>
-      </c>
-      <c r="L14" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="27"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="27"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
-      <c r="W14" s="25" t="s">
+      <c r="O14" s="66" cm="1">
+        <f t="array" aca="1" ref="O14" ca="1">N14/_FV(I14,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="22"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="X14" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="37">
+      <c r="AA14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AC14" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z14" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="8">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="15" spans="1:27" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="22" t="e" vm="13">
+    <row r="15" spans="1:30" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="19" t="e" vm="25">
         <v>#VALUE!</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="5">
-        <v>0</v>
-      </c>
-      <c r="E15" s="37">
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="57">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0</v>
+      </c>
+      <c r="G15" s="50">
+        <f>E15-F15</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="61" cm="1">
+        <f t="array" aca="1" ref="H15" ca="1">G15/_FV(B15,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="53" t="e" vm="26">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J15" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F15" s="7">
-        <v>0</v>
-      </c>
-      <c r="G15" s="47">
+      <c r="M15" s="9">
+        <v>0</v>
+      </c>
+      <c r="N15" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="66" cm="1">
+        <f t="array" aca="1" ref="O15" ca="1">N15/_FV(I15,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="22"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AC15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="19" t="e" vm="27">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.111</v>
+      </c>
+      <c r="E16" s="57">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="5">
-        <v>0</v>
-      </c>
-      <c r="J15" s="50">
+        <v>5550</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0</v>
+      </c>
+      <c r="G16" s="50">
+        <f>E16-F16</f>
+        <v>5550</v>
+      </c>
+      <c r="H16" s="61" cm="1">
+        <f t="array" aca="1" ref="H16" ca="1">G16/_FV(B16,"Price")</f>
+        <v>33.472046318074902</v>
+      </c>
+      <c r="I16" s="53" t="e" vm="28">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J16" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0</v>
+      </c>
+      <c r="L16" s="60">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="9">
+        <v>0</v>
+      </c>
+      <c r="N16" s="59">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K15" s="10">
-        <v>0</v>
-      </c>
-      <c r="L15" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M15" s="27"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="27"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
-      <c r="W15" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="X15" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="37">
+      <c r="O16" s="66" cm="1">
+        <f t="array" aca="1" ref="O16" ca="1">N16/_FV(I16,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="22"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AC16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z15" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="8">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="16" spans="1:27" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="22" t="e" vm="14">
+    <row r="17" spans="1:30" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="19" t="e" vm="29">
         <v>#VALUE!</v>
       </c>
-      <c r="C16" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="5">
+      <c r="C17" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="57">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0</v>
+      </c>
+      <c r="G17" s="50">
+        <f>E17-F17</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="61" cm="1">
+        <f t="array" aca="1" ref="H17" ca="1">G17/_FV(B17,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="53" t="e" vm="30">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J17" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
+      <c r="L17" s="60">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="9">
+        <v>0</v>
+      </c>
+      <c r="N17" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="66" cm="1">
+        <f t="array" aca="1" ref="O17" ca="1">N17/_FV(I17,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="22"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AC17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="3"/>
+      <c r="B18" s="19" t="e" vm="31">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="57">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0</v>
+      </c>
+      <c r="G18" s="50">
+        <f>E18-F18</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="61" cm="1">
+        <f t="array" aca="1" ref="H18" ca="1">G18/_FV(B18,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="53" t="e" vm="32">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J18" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="K18" s="10">
         <v>0.111</v>
       </c>
-      <c r="E16" s="37">
+      <c r="L18" s="14">
         <f t="shared" si="1"/>
         <v>5550</v>
       </c>
-      <c r="F16" s="7">
-        <v>0</v>
-      </c>
-      <c r="G16" s="47">
-        <f t="shared" si="0"/>
-        <v>5550</v>
-      </c>
-      <c r="H16" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="I16" s="5">
-        <v>0</v>
-      </c>
-      <c r="J16" s="50">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="10">
-        <v>0</v>
-      </c>
-      <c r="L16" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="27"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
-      <c r="W16" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="X16" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="37">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z16" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="8">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="22" t="e" vm="15">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0</v>
-      </c>
-      <c r="E17" s="37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="7">
-        <v>0</v>
-      </c>
-      <c r="G17" s="47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="I17" s="5">
-        <v>0</v>
-      </c>
-      <c r="J17" s="50">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="10">
-        <v>0</v>
-      </c>
-      <c r="L17" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M17" s="27"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="X17" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="37">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z17" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="8">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="22" t="e" vm="16">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0</v>
-      </c>
-      <c r="E18" s="37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="7">
-        <v>0</v>
-      </c>
-      <c r="G18" s="47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="I18" s="12">
-        <v>0.111</v>
-      </c>
-      <c r="J18" s="16">
+      <c r="M18" s="15">
+        <v>0</v>
+      </c>
+      <c r="N18" s="67">
         <f t="shared" si="2"/>
         <v>5550</v>
       </c>
-      <c r="K18" s="17">
-        <v>0</v>
-      </c>
-      <c r="L18" s="18">
-        <f t="shared" si="3"/>
-        <v>5550</v>
-      </c>
-      <c r="M18" s="27"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="27"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="25" t="s">
+      <c r="O18" s="68" cm="1">
+        <f t="array" aca="1" ref="O18" ca="1">N18/_FV(I18,"Price")</f>
+        <v>85.070508890251389</v>
+      </c>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="22"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="X18" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="37">
+      <c r="AA18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AC18" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z18" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="8">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="19" spans="1:28" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="23" t="e" vm="17">
+    <row r="19" spans="1:30" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="3"/>
+      <c r="B19" s="20" t="e" vm="33">
         <v>#VALUE!</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="10">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="E19" s="13">
-        <f t="shared" si="1"/>
-        <v>2700</v>
-      </c>
-      <c r="F19" s="14">
-        <v>0</v>
-      </c>
-      <c r="G19" s="15">
+      <c r="E19" s="11">
         <f t="shared" si="0"/>
         <v>2700</v>
       </c>
-      <c r="H19" s="27"/>
-      <c r="I19" s="19">
-        <f>SUM(I3:I18)</f>
-        <v>0.502</v>
-      </c>
-      <c r="J19" s="9"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="43" t="s">
+      <c r="F19" s="12">
+        <v>0</v>
+      </c>
+      <c r="G19" s="58">
+        <f>E19-F19</f>
+        <v>2700</v>
+      </c>
+      <c r="H19" s="62" cm="1">
+        <f t="array" aca="1" ref="H19" ca="1">G19/_FV(B19,"Price")</f>
+        <v>36.571143742203233</v>
+      </c>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="N19" s="44"/>
-      <c r="O19" s="44"/>
-      <c r="P19" s="44"/>
       <c r="Q19" s="45"/>
-      <c r="R19" s="27"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="25" t="s">
+      <c r="R19" s="45"/>
+      <c r="S19" s="45"/>
+      <c r="T19" s="46"/>
+      <c r="U19" s="22"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="X19" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="37">
+      <c r="AA19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AC19" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z19" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="8">
+    </row>
+    <row r="20" spans="1:30" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="D20" s="16"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z20" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="5">
+        <f t="shared" ref="AB20:AB22" si="9">AA20*$A$2</f>
+        <v>0</v>
+      </c>
+      <c r="AC20" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="7">
+        <f t="shared" ref="AD20:AD22" si="10">AB20-AC20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="P21" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>0</v>
+      </c>
+      <c r="R21" s="5">
+        <f>Q21*$A$2</f>
+        <v>0</v>
+      </c>
+      <c r="S21" s="6">
+        <v>0</v>
+      </c>
+      <c r="T21" s="7">
+        <f>R21-S21</f>
+        <v>0</v>
+      </c>
+      <c r="Z21" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AC21" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="7">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:28" ht="18" x14ac:dyDescent="0.25">
-      <c r="D20" s="19"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q20" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="W20" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="X20" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="37">
-        <f t="shared" ref="Y20:Y22" si="10">X20*$A$2</f>
-        <v>0</v>
-      </c>
-      <c r="Z20" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="8">
-        <f t="shared" ref="AA20:AA22" si="11">Y20-Z20</f>
+    <row r="22" spans="1:30" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P22" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>0</v>
+      </c>
+      <c r="R22" s="5">
+        <f t="shared" ref="R22:R25" si="11">Q22*$A$2</f>
+        <v>0</v>
+      </c>
+      <c r="S22" s="6">
+        <v>0</v>
+      </c>
+      <c r="T22" s="7">
+        <f t="shared" ref="T22:T25" si="12">R22-S22</f>
+        <v>0</v>
+      </c>
+      <c r="Z22" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA22" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AC22" s="12">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="13">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="18" x14ac:dyDescent="0.25">
-      <c r="M21" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="N21" s="5">
-        <v>0</v>
-      </c>
-      <c r="O21" s="6">
-        <f>N21*$A$2</f>
-        <v>0</v>
-      </c>
-      <c r="P21" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="8">
-        <f>O21-P21</f>
-        <v>0</v>
-      </c>
-      <c r="W21" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="X21" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="37">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Z21" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA21" s="8">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M22" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="N22" s="5">
-        <v>0</v>
-      </c>
-      <c r="O22" s="6">
-        <f t="shared" ref="O22:O25" si="12">N22*$A$2</f>
-        <v>0</v>
-      </c>
-      <c r="P22" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="8">
-        <f t="shared" ref="Q22:Q25" si="13">O22-P22</f>
-        <v>0</v>
-      </c>
-      <c r="W22" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="X22" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="13">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Z22" s="14">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="15">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28" ht="18" x14ac:dyDescent="0.25">
-      <c r="C23" s="52" t="s">
+    <row r="23" spans="1:30" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C23" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="34">
+      <c r="D23" s="38">
         <f>SUM(D3:D19)</f>
         <v>0.26</v>
       </c>
-      <c r="M23" s="25" t="s">
+      <c r="P23" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="N23" s="5">
-        <v>0</v>
-      </c>
-      <c r="O23" s="6">
+      <c r="Q23" s="4">
+        <v>0</v>
+      </c>
+      <c r="R23" s="5">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="S23" s="6">
+        <v>0</v>
+      </c>
+      <c r="T23" s="7">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P23" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="8">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="W23" s="38"/>
-      <c r="X23" s="34"/>
-      <c r="Y23" s="39"/>
-      <c r="Z23" s="35"/>
-      <c r="AA23" s="39"/>
-      <c r="AB23" s="40"/>
+      <c r="AA23" s="26"/>
+      <c r="AB23" s="5"/>
+      <c r="AC23" s="27"/>
+      <c r="AD23" s="5"/>
     </row>
-    <row r="24" spans="1:28" ht="18" x14ac:dyDescent="0.25">
-      <c r="C24" s="52" t="s">
+    <row r="24" spans="1:30" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C24" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="34">
-        <f>SUM(I3:I18)</f>
+      <c r="D24" s="38">
+        <f>SUM(K3:K18)</f>
         <v>0.502</v>
       </c>
-      <c r="M24" s="25" t="s">
+      <c r="P24" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="N24" s="5">
-        <v>0</v>
-      </c>
-      <c r="O24" s="6">
+      <c r="Q24" s="4">
+        <v>0</v>
+      </c>
+      <c r="R24" s="5">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="S24" s="6">
+        <v>0</v>
+      </c>
+      <c r="T24" s="7">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P24" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="8">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="W24" s="38"/>
-      <c r="X24" s="34"/>
-      <c r="Y24" s="39"/>
-      <c r="Z24" s="35"/>
-      <c r="AA24" s="39"/>
-      <c r="AB24" s="40"/>
+      <c r="AA24" s="26"/>
+      <c r="AB24" s="5"/>
+      <c r="AC24" s="27"/>
+      <c r="AD24" s="5"/>
     </row>
-    <row r="25" spans="1:28" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="52" t="s">
+    <row r="25" spans="1:30" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="D25" s="34">
-        <f>SUM(N3:N9)</f>
+      <c r="D25" s="38">
+        <f>SUM(Q3:Q9)</f>
         <v>0.184</v>
       </c>
-      <c r="M25" s="26" t="s">
+      <c r="P25" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="N25" s="12">
-        <v>0</v>
-      </c>
-      <c r="O25" s="13">
+      <c r="Q25" s="10">
+        <v>0</v>
+      </c>
+      <c r="R25" s="11">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="S25" s="12">
+        <v>0</v>
+      </c>
+      <c r="T25" s="13">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P25" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="15">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="26" spans="1:28" ht="18" x14ac:dyDescent="0.25">
-      <c r="C26" s="52" t="s">
+    <row r="26" spans="1:30" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C26" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="34">
-        <f>SUM(S3:S8)</f>
+      <c r="D26" s="38">
+        <f>SUM(V3:V8)</f>
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="18" x14ac:dyDescent="0.25">
-      <c r="C27" s="52" t="s">
+    <row r="27" spans="1:30" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C27" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="D27" s="34">
-        <f>SUM(X3:X22)</f>
+      <c r="D27" s="38">
+        <f>SUM(AA3:AA22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="18" x14ac:dyDescent="0.25">
-      <c r="C28" s="52" t="s">
+    <row r="28" spans="1:30" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C28" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="34">
+      <c r="D28" s="38">
         <f>A10</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="P19:T19"/>
+    <mergeCell ref="Z1:AD1"/>
     <mergeCell ref="C1:G1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="R1:V1"/>
-    <mergeCell ref="M19:Q19"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="U1:Y1"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="V3:V8 Q3:Q9 G3:G19 Q21:Q25 AA3:AA24 L3:L18">
+  <conditionalFormatting sqref="Y3:Y8 T3:T9 AD3:AD24 T21:T25 G3:H19 N3:O18">
     <cfRule type="cellIs" dxfId="1" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>